<commit_message>
Implemented click and site selection
</commit_message>
<xml_diff>
--- a/data/flux_site_loc.xlsx
+++ b/data/flux_site_loc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26605"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2b57\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dennis\Duke\Data+\Quantifying-wetland-carbon-emissions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A00817A9-EA79-4E31-BF8D-7DA4423E4F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90DA2B4-473E-40FF-8778-14C40BDF2AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -917,11 +917,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -932,7 +934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -943,7 +945,7 @@
         <v>28.052099999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -954,7 +956,7 @@
         <v>25.5519</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -965,7 +967,7 @@
         <v>25.437899999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -976,7 +978,7 @@
         <v>33.345500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -987,7 +989,7 @@
         <v>28.708400000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>29.501300000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1009,7 +1011,7 @@
         <v>29.858699999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>35.811799999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1031,7 +1033,7 @@
         <v>35.802999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1042,7 +1044,7 @@
         <v>35.7879</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>

</xml_diff>